<commit_message>
Added tesst page for Russell
</commit_message>
<xml_diff>
--- a/Project Data/Sample Proj/4304.xlsx
+++ b/Project Data/Sample Proj/4304.xlsx
@@ -183,7 +183,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +194,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -227,13 +233,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -553,7 +559,7 @@
     <col min="1" max="1" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="16.290714285714284" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>

</xml_diff>